<commit_message>
Calculate current that is being outputted
</commit_message>
<xml_diff>
--- a/Documents/NegativeVoltageMuliplier555.xlsx
+++ b/Documents/NegativeVoltageMuliplier555.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{223AA12A-77DB-4D07-8F92-F580D927269B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5DDB81-4F0B-427D-8C60-4B639FF8EF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6B13671-B74D-4B32-97AC-33BB8C89940B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>RA</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Sim</t>
+  </si>
+  <si>
+    <t>Io (NL)</t>
+  </si>
+  <si>
+    <t>Io at 1k (mA)</t>
+  </si>
+  <si>
+    <t>Io at 470 (mA)</t>
   </si>
 </sst>
 </file>
@@ -432,18 +441,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B1AFC1-D49D-419D-9A69-C099542424C0}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:L6"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -477,8 +488,17 @@
       <c r="L1" t="s">
         <v>9</v>
       </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>470</v>
       </c>
@@ -515,7 +535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1500</v>
       </c>
@@ -546,7 +566,7 @@
         <v>0.53488372093023251</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -588,8 +608,19 @@
       <c r="L4">
         <v>-8.18</v>
       </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>1000*K4/1000</f>
+        <v>-11.14</v>
+      </c>
+      <c r="O4">
+        <f>1000*L4/470</f>
+        <v>-17.404255319148938</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -631,8 +662,16 @@
       <c r="L5">
         <v>-12.2</v>
       </c>
+      <c r="N5">
+        <f>1000*K5/1000</f>
+        <v>-13.7</v>
+      </c>
+      <c r="O5">
+        <f>1000*L5/470</f>
+        <v>-25.957446808510639</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="J6">
         <f>J4-J5</f>
         <v>2.8800000000000008</v>

</xml_diff>